<commit_message>
propper Serial Comand System added
</commit_message>
<xml_diff>
--- a/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
+++ b/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgewi\Documents\Fynn\Projekte\Balloon\SpiCy-BEXUS\micorcontroller\Hardware\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3026F924-D145-4F0E-A49B-EFE7BD696065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83683B63-A460-44A4-8398-81CB5F3B9D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF6BBEE3-69E0-44E7-9484-437EE6090CBD}"/>
   </bookViews>
@@ -369,7 +369,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -407,6 +407,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Akzent1" xfId="2" builtinId="30"/>
@@ -566,22 +567,22 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -593,67 +594,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.38559994139171649</c:v>
+                  <c:v>9.7057622154934596E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48240941437347984</c:v>
+                  <c:v>1.2598343170930336E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59355178262034647</c:v>
+                  <c:v>1.6199026494879216E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71815010702712501</c:v>
+                  <c:v>2.0641773750447085E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.85447189875940566</c:v>
+                  <c:v>2.6077262528154194E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>3.2673267326732675E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1516186418096925</c:v>
+                  <c:v>4.0614658906958374E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3058875379879644</c:v>
+                  <c:v>5.0102932076940214E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4593540628722756</c:v>
+                  <c:v>6.1355167729016405E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6088458138274524</c:v>
+                  <c:v>7.4602334994228317E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7516955373117613</c:v>
+                  <c:v>9.0086845259037457E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.8858722365733001</c:v>
+                  <c:v>0.10805928325461811</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.010016888292057</c:v>
+                  <c:v>0.1287742631616135</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1234002012423638</c:v>
+                  <c:v>0.15248539102088868</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.2258292517918932</c:v>
+                  <c:v>0.17943935939032254</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3175302095323866</c:v>
+                  <c:v>0.24398723123301194</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.3990289515203256</c:v>
+                  <c:v>0.42041498309160763</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.4710437850520233</c:v>
+                  <c:v>1.1208813163169407</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5343973964105437</c:v>
+                  <c:v>1.9185089414779546</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.5899498144026194</c:v>
+                  <c:v>2.4953196431987865</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.6385508675844984</c:v>
+                  <c:v>2.8298416372353588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -680,7 +681,6 @@
         <c:axId val="1669192655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -991,22 +991,22 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1018,67 +1018,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>33900.420850329079</c:v>
+                  <c:v>339004.20850329078</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26093.920543571829</c:v>
+                  <c:v>260939.20543571829</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20271.594558742065</c:v>
+                  <c:v>202715.94558742066</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15886.998210018286</c:v>
+                  <c:v>158869.98210018285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12554.70252652927</c:v>
+                  <c:v>125547.02526529272</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8025.1451786404677</c:v>
+                  <c:v>80251.451786404679</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6486.4408792131726</c:v>
+                  <c:v>64864.408792131726</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5278.5200532331801</c:v>
+                  <c:v>52785.200532331801</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4323.4540383425092</c:v>
+                  <c:v>43234.540383425097</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3563.1319373112869</c:v>
+                  <c:v>35631.31937311287</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2953.8792231522302</c:v>
+                  <c:v>29538.792231522304</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2462.6238651883828</c:v>
+                  <c:v>24626.238651883828</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2064.1417436165666</c:v>
+                  <c:v>20641.417436165666</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1739.0614028117036</c:v>
+                  <c:v>17390.614028117034</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1472.4075389837451</c:v>
+                  <c:v>12525.297956467419</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1252.5297956467418</c:v>
+                  <c:v>6849.3872309991775</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1070.3092720326706</c:v>
+                  <c:v>1944.1118805007284</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>918.56668620494838</c:v>
+                  <c:v>720.08580656277297</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>791.61801382618705</c:v>
+                  <c:v>322.47586356098327</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>684.93872309991775</c:v>
+                  <c:v>166.14299421502844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,7 +1105,6 @@
         <c:axId val="1665994287"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1168,7 +1167,6 @@
         <c:axId val="1665990927"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="30000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1407,22 +1405,22 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>100</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1434,67 +1432,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-2.8800117216567056E-2</c:v>
+                  <c:v>-0.78058847556901312</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16481882874695963</c:v>
+                  <c:v>-0.77480331365813937</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38710356524069289</c:v>
+                  <c:v>-0.76760194701024165</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63630021405424997</c:v>
+                  <c:v>-0.75871645249910591</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90894379751881127</c:v>
+                  <c:v>-0.74784547494369169</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2</c:v>
+                  <c:v>-0.73465346534653464</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.503237283619385</c:v>
+                  <c:v>-0.71877068218608331</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8117750759759288</c:v>
+                  <c:v>-0.6997941358461196</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.1187081257445515</c:v>
+                  <c:v>-0.67728966454196726</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4176916276549045</c:v>
+                  <c:v>-0.65079533001154344</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.7033910746235223</c:v>
+                  <c:v>-0.61982630948192519</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9717444731466003</c:v>
+                  <c:v>-0.58388143349076382</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2200337765841143</c:v>
+                  <c:v>-0.54245147367677304</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.4468004024847279</c:v>
+                  <c:v>-0.49502921795822269</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6516585035837865</c:v>
+                  <c:v>-0.44112128121935495</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.8350604190647735</c:v>
+                  <c:v>-0.31202553753397616</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.9980579030406513</c:v>
+                  <c:v>4.0829966183215216E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.1420875701040467</c:v>
+                  <c:v>1.4417626326338813</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.2687947928210876</c:v>
+                  <c:v>3.0370178829559089</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.379899628805239</c:v>
+                  <c:v>4.1906392863975732</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.477101735168997</c:v>
+                  <c:v>4.8596832744707177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4016,8 +4014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F92C7C-F2BA-463C-A1E4-8CB622B0EF6B}">
   <dimension ref="B1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="83" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="75" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4115,7 +4113,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="26">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -4124,7 +4122,7 @@
       </c>
       <c r="H6" s="26">
         <f t="shared" ref="H6:H26" si="0">D$6*EXP(D$5*(1/(G6+273.15)-1/298.15))</f>
-        <v>33900.420850329079</v>
+        <v>339004.20850329078</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -4147,7 +4145,7 @@
       </c>
       <c r="H7" s="26">
         <f t="shared" si="0"/>
-        <v>26093.920543571829</v>
+        <v>260939.20543571829</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -4170,7 +4168,7 @@
       </c>
       <c r="H8" s="26">
         <f t="shared" si="0"/>
-        <v>20271.594558742065</v>
+        <v>202715.94558742066</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -4193,7 +4191,7 @@
       </c>
       <c r="H9" s="26">
         <f t="shared" si="0"/>
-        <v>15886.998210018286</v>
+        <v>158869.98210018285</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -4216,7 +4214,7 @@
       </c>
       <c r="H10" s="26">
         <f t="shared" si="0"/>
-        <v>12554.70252652927</v>
+        <v>125547.02526529272</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -4241,7 +4239,7 @@
       </c>
       <c r="H11" s="26">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -4264,7 +4262,7 @@
       </c>
       <c r="H12" s="26">
         <f t="shared" si="0"/>
-        <v>8025.1451786404677</v>
+        <v>80251.451786404679</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -4287,7 +4285,7 @@
       </c>
       <c r="H13" s="26">
         <f t="shared" si="0"/>
-        <v>6486.4408792131726</v>
+        <v>64864.408792131726</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -4310,7 +4308,7 @@
       </c>
       <c r="H14" s="26">
         <f t="shared" si="0"/>
-        <v>5278.5200532331801</v>
+        <v>52785.200532331801</v>
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -4333,7 +4331,7 @@
       </c>
       <c r="H15" s="26">
         <f t="shared" si="0"/>
-        <v>4323.4540383425092</v>
+        <v>43234.540383425097</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -4356,7 +4354,7 @@
       </c>
       <c r="H16" s="26">
         <f t="shared" si="0"/>
-        <v>3563.1319373112869</v>
+        <v>35631.31937311287</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -4379,7 +4377,7 @@
       </c>
       <c r="H17" s="26">
         <f t="shared" si="0"/>
-        <v>2953.8792231522302</v>
+        <v>29538.792231522304</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -4402,7 +4400,7 @@
       </c>
       <c r="H18" s="26">
         <f t="shared" si="0"/>
-        <v>2462.6238651883828</v>
+        <v>24626.238651883828</v>
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -4427,7 +4425,7 @@
       </c>
       <c r="H19" s="26">
         <f t="shared" si="0"/>
-        <v>2064.1417436165666</v>
+        <v>20641.417436165666</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -4450,7 +4448,7 @@
       </c>
       <c r="H20" s="26">
         <f t="shared" si="0"/>
-        <v>1739.0614028117036</v>
+        <v>17390.614028117034</v>
       </c>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -4468,12 +4466,11 @@
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="26">
-        <f t="shared" si="1"/>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H21" s="26">
         <f t="shared" si="0"/>
-        <v>1472.4075389837451</v>
+        <v>12525.297956467419</v>
       </c>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -4491,12 +4488,11 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="26">
-        <f>G21+5</f>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H22" s="26">
         <f t="shared" si="0"/>
-        <v>1252.5297956467418</v>
+        <v>6849.3872309991775</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -4514,12 +4510,11 @@
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="26">
-        <f t="shared" si="1"/>
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="H23" s="26">
         <f t="shared" si="0"/>
-        <v>1070.3092720326706</v>
+        <v>1944.1118805007284</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -4537,12 +4532,11 @@
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="26">
-        <f t="shared" si="1"/>
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="H24" s="26">
         <f t="shared" si="0"/>
-        <v>918.56668620494838</v>
+        <v>720.08580656277297</v>
       </c>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -4560,12 +4554,11 @@
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="26">
-        <f t="shared" si="1"/>
-        <v>95</v>
+        <v>250</v>
       </c>
       <c r="H25" s="26">
         <f t="shared" si="0"/>
-        <v>791.61801382618705</v>
+        <v>322.47586356098327</v>
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -4583,12 +4576,11 @@
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="26">
-        <f>G25+5</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="H26" s="26">
         <f t="shared" si="0"/>
-        <v>684.93872309991775</v>
+        <v>166.14299421502844</v>
       </c>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -4706,7 +4698,7 @@
       </c>
       <c r="J33" s="26">
         <f>D34/(D35+H26)*1000</f>
-        <v>0.52771017351689964</v>
+        <v>2.8298416372353588</v>
       </c>
       <c r="K33" s="22"/>
       <c r="L33" s="20"/>
@@ -4720,8 +4712,8 @@
       <c r="C34" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="26">
-        <v>3</v>
+      <c r="D34" s="31">
+        <v>3.3</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="26">
@@ -4730,7 +4722,7 @@
       </c>
       <c r="G34" s="26">
         <f>D$34*(D$35/(D$35+H6))</f>
-        <v>0.38559994139171649</v>
+        <v>9.7057622154934596E-3</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="26" t="s">
@@ -4738,7 +4730,7 @@
       </c>
       <c r="J34" s="26">
         <f>1000*D34/(D35+H12)</f>
-        <v>0.23032372836193848</v>
+        <v>4.0614658906958374E-2</v>
       </c>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
@@ -4753,7 +4745,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="26">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="26">
@@ -4762,7 +4754,7 @@
       </c>
       <c r="G35" s="26">
         <f t="shared" ref="G35:G54" si="3">D$34*(D$35/(D$35+H7))</f>
-        <v>0.48240941437347984</v>
+        <v>1.2598343170930336E-2</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="26" t="s">
@@ -4770,7 +4762,7 @@
       </c>
       <c r="J35" s="26">
         <f>1000*(G41-G39)/10</f>
-        <v>30.588753798796443</v>
+        <v>1.7429664750207539</v>
       </c>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
@@ -4790,7 +4782,7 @@
       </c>
       <c r="G36" s="26">
         <f t="shared" si="3"/>
-        <v>0.59355178262034647</v>
+        <v>1.6199026494879216E-2</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="26" t="s">
@@ -4818,7 +4810,7 @@
       </c>
       <c r="G37" s="26">
         <f t="shared" si="3"/>
-        <v>0.71815010702712501</v>
+        <v>2.0641773750447085E-2</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="26" t="s">
@@ -4826,7 +4818,7 @@
       </c>
       <c r="J37" s="26">
         <f>J36/J35</f>
-        <v>2.3944155417956848E-2</v>
+        <v>0.42021569863601588</v>
       </c>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
@@ -4846,7 +4838,7 @@
       </c>
       <c r="G38" s="26">
         <f t="shared" si="3"/>
-        <v>0.85447189875940566</v>
+        <v>2.6077262528154194E-2</v>
       </c>
       <c r="H38" s="22"/>
       <c r="I38" s="20"/>
@@ -4869,7 +4861,7 @@
       </c>
       <c r="G39" s="26">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3.2673267326732675E-2</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="20"/>
@@ -4892,7 +4884,7 @@
       </c>
       <c r="G40" s="26">
         <f t="shared" si="3"/>
-        <v>1.1516186418096925</v>
+        <v>4.0614658906958374E-2</v>
       </c>
       <c r="H40" s="22"/>
       <c r="I40" s="20"/>
@@ -4915,7 +4907,7 @@
       </c>
       <c r="G41" s="26">
         <f t="shared" si="3"/>
-        <v>1.3058875379879644</v>
+        <v>5.0102932076940214E-2</v>
       </c>
       <c r="H41" s="22"/>
       <c r="I41" s="20"/>
@@ -4938,7 +4930,7 @@
       </c>
       <c r="G42" s="26">
         <f t="shared" si="3"/>
-        <v>1.4593540628722756</v>
+        <v>6.1355167729016405E-2</v>
       </c>
       <c r="H42" s="22"/>
       <c r="I42" s="20"/>
@@ -4961,7 +4953,7 @@
       </c>
       <c r="G43" s="26">
         <f t="shared" si="3"/>
-        <v>1.6088458138274524</v>
+        <v>7.4602334994228317E-2</v>
       </c>
       <c r="H43" s="22"/>
       <c r="I43" s="20"/>
@@ -4984,7 +4976,7 @@
       </c>
       <c r="G44" s="26">
         <f t="shared" si="3"/>
-        <v>1.7516955373117613</v>
+        <v>9.0086845259037457E-2</v>
       </c>
       <c r="H44" s="22"/>
       <c r="I44" s="20"/>
@@ -5007,7 +4999,7 @@
       </c>
       <c r="G45" s="26">
         <f t="shared" si="3"/>
-        <v>1.8858722365733001</v>
+        <v>0.10805928325461811</v>
       </c>
       <c r="H45" s="22"/>
       <c r="I45" s="20"/>
@@ -5030,7 +5022,7 @@
       </c>
       <c r="G46" s="26">
         <f t="shared" si="3"/>
-        <v>2.010016888292057</v>
+        <v>0.1287742631616135</v>
       </c>
       <c r="H46" s="22"/>
       <c r="I46" s="20"/>
@@ -5053,7 +5045,7 @@
       </c>
       <c r="G47" s="26">
         <f t="shared" si="3"/>
-        <v>2.1234002012423638</v>
+        <v>0.15248539102088868</v>
       </c>
       <c r="H47" s="22"/>
       <c r="I47" s="20"/>
@@ -5076,7 +5068,7 @@
       </c>
       <c r="G48" s="26">
         <f t="shared" si="3"/>
-        <v>2.2258292517918932</v>
+        <v>0.17943935939032254</v>
       </c>
       <c r="H48" s="22"/>
       <c r="I48" s="20"/>
@@ -5095,11 +5087,11 @@
       <c r="E49" s="20"/>
       <c r="F49" s="26">
         <f t="shared" ref="F49" si="17">G21</f>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G49" s="26">
         <f>D$34*(D$35/(D$35+H21))</f>
-        <v>2.3175302095323866</v>
+        <v>0.24398723123301194</v>
       </c>
       <c r="H49" s="22"/>
       <c r="I49" s="20"/>
@@ -5118,11 +5110,11 @@
       <c r="E50" s="20"/>
       <c r="F50" s="26">
         <f t="shared" ref="F50" si="18">G22</f>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G50" s="26">
         <f t="shared" si="3"/>
-        <v>2.3990289515203256</v>
+        <v>0.42041498309160763</v>
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="20"/>
@@ -5141,11 +5133,11 @@
       <c r="E51" s="20"/>
       <c r="F51" s="26">
         <f t="shared" ref="F51" si="19">G23</f>
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="G51" s="26">
         <f t="shared" si="3"/>
-        <v>2.4710437850520233</v>
+        <v>1.1208813163169407</v>
       </c>
       <c r="H51" s="22"/>
       <c r="I51" s="20"/>
@@ -5164,11 +5156,11 @@
       <c r="E52" s="20"/>
       <c r="F52" s="26">
         <f>G24</f>
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="G52" s="26">
         <f t="shared" si="3"/>
-        <v>2.5343973964105437</v>
+        <v>1.9185089414779546</v>
       </c>
       <c r="H52" s="22"/>
       <c r="I52" s="20"/>
@@ -5187,11 +5179,11 @@
       <c r="E53" s="20"/>
       <c r="F53" s="26">
         <f t="shared" ref="F53" si="20">G25</f>
-        <v>95</v>
+        <v>250</v>
       </c>
       <c r="G53" s="26">
         <f t="shared" si="3"/>
-        <v>2.5899498144026194</v>
+        <v>2.4953196431987865</v>
       </c>
       <c r="H53" s="22"/>
       <c r="I53" s="20"/>
@@ -5210,11 +5202,11 @@
       <c r="E54" s="20"/>
       <c r="F54" s="26">
         <f t="shared" ref="F54" si="21">G26</f>
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="G54" s="26">
         <f t="shared" si="3"/>
-        <v>2.6385508675844984</v>
+        <v>2.8298416372353588</v>
       </c>
       <c r="H54" s="22"/>
       <c r="I54" s="20"/>
@@ -5329,8 +5321,8 @@
         <v>0</v>
       </c>
       <c r="J60" s="26">
-        <f t="shared" ref="J60:J80" si="22">D$60*(G34-D$61)</f>
-        <v>-2.8800117216567056E-2</v>
+        <f>D$60*(G34-D$61)</f>
+        <v>-0.78058847556901312</v>
       </c>
       <c r="K60" s="8"/>
       <c r="L60" s="26" t="s">
@@ -5364,12 +5356,12 @@
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="26">
-        <f t="shared" ref="I61:I80" si="23">F35</f>
+        <f>F35</f>
         <v>5</v>
       </c>
       <c r="J61" s="26">
-        <f t="shared" si="22"/>
-        <v>0.16481882874695963</v>
+        <f>D$60*(G35-D$61)</f>
+        <v>-0.77480331365813937</v>
       </c>
       <c r="K61" s="8"/>
       <c r="L61" s="26" t="s">
@@ -5377,7 +5369,7 @@
       </c>
       <c r="M61" s="26">
         <f>1000*(J67-J65)/10</f>
-        <v>61.177507597592886</v>
+        <v>3.4859329500415037</v>
       </c>
       <c r="N61" s="26" t="s">
         <v>33</v>
@@ -5403,12 +5395,12 @@
       </c>
       <c r="H62" s="8"/>
       <c r="I62" s="26">
-        <f t="shared" si="23"/>
+        <f>F36</f>
         <v>10</v>
       </c>
       <c r="J62" s="26">
-        <f t="shared" si="22"/>
-        <v>0.38710356524069289</v>
+        <f>D$60*(G36-D$61)</f>
+        <v>-0.76760194701024165</v>
       </c>
       <c r="K62" s="8"/>
       <c r="L62" s="26" t="s">
@@ -5431,19 +5423,19 @@
       </c>
       <c r="D63" s="26">
         <f>D35</f>
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
       <c r="I63" s="26">
-        <f t="shared" si="23"/>
+        <f>F37</f>
         <v>15</v>
       </c>
       <c r="J63" s="26">
-        <f t="shared" si="22"/>
-        <v>0.63630021405424997</v>
+        <f>D$60*(G37-D$61)</f>
+        <v>-0.75871645249910591</v>
       </c>
       <c r="K63" s="8"/>
       <c r="L63" s="26" t="s">
@@ -5451,7 +5443,7 @@
       </c>
       <c r="M63" s="26">
         <f>M62/M61</f>
-        <v>1.1972077708978424E-2</v>
+        <v>0.21010784931800819</v>
       </c>
       <c r="N63" s="26" t="s">
         <v>31</v>
@@ -5474,12 +5466,12 @@
       <c r="G64" s="27"/>
       <c r="H64" s="30"/>
       <c r="I64" s="26">
-        <f t="shared" si="23"/>
+        <f>F38</f>
         <v>20</v>
       </c>
       <c r="J64" s="26">
-        <f t="shared" si="22"/>
-        <v>0.90894379751881127</v>
+        <f>D$60*(G38-D$61)</f>
+        <v>-0.74784547494369169</v>
       </c>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
@@ -5501,12 +5493,12 @@
       <c r="G65" s="27"/>
       <c r="H65" s="30"/>
       <c r="I65" s="26">
-        <f t="shared" si="23"/>
+        <f>F39</f>
         <v>25</v>
       </c>
       <c r="J65" s="26">
-        <f t="shared" si="22"/>
-        <v>1.2</v>
+        <f>D$60*(G39-D$61)</f>
+        <v>-0.73465346534653464</v>
       </c>
       <c r="K65" s="8"/>
       <c r="L65" s="27"/>
@@ -5528,12 +5520,12 @@
       <c r="G66" s="27"/>
       <c r="H66" s="30"/>
       <c r="I66" s="26">
-        <f t="shared" si="23"/>
+        <f>F40</f>
         <v>30</v>
       </c>
       <c r="J66" s="26">
-        <f t="shared" si="22"/>
-        <v>1.503237283619385</v>
+        <f>D$60*(G40-D$61)</f>
+        <v>-0.71877068218608331</v>
       </c>
       <c r="K66" s="8"/>
       <c r="L66" s="27"/>
@@ -5551,12 +5543,12 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
       <c r="I67" s="26">
-        <f t="shared" si="23"/>
+        <f>F41</f>
         <v>35</v>
       </c>
       <c r="J67" s="26">
-        <f t="shared" si="22"/>
-        <v>1.8117750759759288</v>
+        <f>D$60*(G41-D$61)</f>
+        <v>-0.6997941358461196</v>
       </c>
       <c r="K67" s="8"/>
       <c r="L67" s="27"/>
@@ -5576,12 +5568,12 @@
       <c r="G68" s="28"/>
       <c r="H68" s="8"/>
       <c r="I68" s="26">
-        <f t="shared" si="23"/>
+        <f>F42</f>
         <v>40</v>
       </c>
       <c r="J68" s="26">
-        <f t="shared" si="22"/>
-        <v>2.1187081257445515</v>
+        <f>D$60*(G42-D$61)</f>
+        <v>-0.67728966454196726</v>
       </c>
       <c r="K68" s="8"/>
       <c r="L68" s="27"/>
@@ -5599,12 +5591,12 @@
       <c r="G69" s="28"/>
       <c r="H69" s="8"/>
       <c r="I69" s="26">
-        <f t="shared" si="23"/>
+        <f>F43</f>
         <v>45</v>
       </c>
       <c r="J69" s="26">
-        <f t="shared" si="22"/>
-        <v>2.4176916276549045</v>
+        <f>D$60*(G43-D$61)</f>
+        <v>-0.65079533001154344</v>
       </c>
       <c r="K69" s="8"/>
       <c r="L69" s="27"/>
@@ -5622,12 +5614,12 @@
       <c r="G70" s="28"/>
       <c r="H70" s="8"/>
       <c r="I70" s="26">
-        <f t="shared" si="23"/>
+        <f>F44</f>
         <v>50</v>
       </c>
       <c r="J70" s="26">
-        <f t="shared" si="22"/>
-        <v>2.7033910746235223</v>
+        <f>D$60*(G44-D$61)</f>
+        <v>-0.61982630948192519</v>
       </c>
       <c r="K70" s="8"/>
       <c r="L70" s="27"/>
@@ -5645,12 +5637,12 @@
       <c r="G71" s="28"/>
       <c r="H71" s="8"/>
       <c r="I71" s="26">
-        <f t="shared" si="23"/>
+        <f>F45</f>
         <v>55</v>
       </c>
       <c r="J71" s="26">
-        <f t="shared" si="22"/>
-        <v>2.9717444731466003</v>
+        <f>D$60*(G45-D$61)</f>
+        <v>-0.58388143349076382</v>
       </c>
       <c r="K71" s="8"/>
       <c r="L71" s="27"/>
@@ -5668,12 +5660,12 @@
       <c r="G72" s="28"/>
       <c r="H72" s="8"/>
       <c r="I72" s="26">
-        <f t="shared" si="23"/>
+        <f>F46</f>
         <v>60</v>
       </c>
       <c r="J72" s="26">
-        <f t="shared" si="22"/>
-        <v>3.2200337765841143</v>
+        <f>D$60*(G46-D$61)</f>
+        <v>-0.54245147367677304</v>
       </c>
       <c r="K72" s="8"/>
       <c r="L72" s="27"/>
@@ -5691,12 +5683,12 @@
       <c r="G73" s="28"/>
       <c r="H73" s="8"/>
       <c r="I73" s="26">
-        <f t="shared" si="23"/>
+        <f>F47</f>
         <v>65</v>
       </c>
       <c r="J73" s="26">
-        <f t="shared" si="22"/>
-        <v>3.4468004024847279</v>
+        <f>D$60*(G47-D$61)</f>
+        <v>-0.49502921795822269</v>
       </c>
       <c r="K73" s="8"/>
       <c r="L73" s="27"/>
@@ -5714,12 +5706,12 @@
       <c r="G74" s="28"/>
       <c r="H74" s="8"/>
       <c r="I74" s="26">
-        <f t="shared" si="23"/>
+        <f>F48</f>
         <v>70</v>
       </c>
       <c r="J74" s="26">
-        <f t="shared" si="22"/>
-        <v>3.6516585035837865</v>
+        <f>D$60*(G48-D$61)</f>
+        <v>-0.44112128121935495</v>
       </c>
       <c r="K74" s="8"/>
       <c r="L74" s="27"/>
@@ -5737,12 +5729,12 @@
       <c r="G75" s="28"/>
       <c r="H75" s="8"/>
       <c r="I75" s="26">
-        <f t="shared" si="23"/>
-        <v>75</v>
+        <f>F49</f>
+        <v>80</v>
       </c>
       <c r="J75" s="26">
-        <f t="shared" si="22"/>
-        <v>3.8350604190647735</v>
+        <f>D$60*(G49-D$61)</f>
+        <v>-0.31202553753397616</v>
       </c>
       <c r="K75" s="8"/>
       <c r="L75" s="27"/>
@@ -5760,12 +5752,12 @@
       <c r="G76" s="28"/>
       <c r="H76" s="8"/>
       <c r="I76" s="26">
-        <f t="shared" si="23"/>
-        <v>80</v>
+        <f>F50</f>
+        <v>100</v>
       </c>
       <c r="J76" s="26">
-        <f t="shared" si="22"/>
-        <v>3.9980579030406513</v>
+        <f>D$60*(G50-D$61)</f>
+        <v>4.0829966183215216E-2</v>
       </c>
       <c r="K76" s="8"/>
       <c r="L76" s="27"/>
@@ -5783,12 +5775,12 @@
       <c r="G77" s="28"/>
       <c r="H77" s="8"/>
       <c r="I77" s="26">
-        <f t="shared" si="23"/>
-        <v>85</v>
+        <f>F51</f>
+        <v>150</v>
       </c>
       <c r="J77" s="26">
-        <f t="shared" si="22"/>
-        <v>4.1420875701040467</v>
+        <f>D$60*(G51-D$61)</f>
+        <v>1.4417626326338813</v>
       </c>
       <c r="K77" s="8"/>
       <c r="L77" s="27"/>
@@ -5806,12 +5798,12 @@
       <c r="G78" s="28"/>
       <c r="H78" s="8"/>
       <c r="I78" s="26">
-        <f t="shared" si="23"/>
-        <v>90</v>
+        <f>F52</f>
+        <v>200</v>
       </c>
       <c r="J78" s="26">
-        <f t="shared" si="22"/>
-        <v>4.2687947928210876</v>
+        <f>D$60*(G52-D$61)</f>
+        <v>3.0370178829559089</v>
       </c>
       <c r="K78" s="8"/>
       <c r="L78" s="27"/>
@@ -5829,12 +5821,12 @@
       <c r="G79" s="28"/>
       <c r="H79" s="8"/>
       <c r="I79" s="26">
-        <f t="shared" si="23"/>
-        <v>95</v>
+        <f>F53</f>
+        <v>250</v>
       </c>
       <c r="J79" s="26">
-        <f t="shared" si="22"/>
-        <v>4.379899628805239</v>
+        <f>D$60*(G53-D$61)</f>
+        <v>4.1906392863975732</v>
       </c>
       <c r="K79" s="8"/>
       <c r="L79" s="27"/>
@@ -5852,12 +5844,12 @@
       <c r="G80" s="28"/>
       <c r="H80" s="8"/>
       <c r="I80" s="26">
-        <f t="shared" si="23"/>
-        <v>100</v>
+        <f>F54</f>
+        <v>300</v>
       </c>
       <c r="J80" s="26">
-        <f t="shared" si="22"/>
-        <v>4.477101735168997</v>
+        <f>D$60*(G54-D$61)</f>
+        <v>4.8596832744707177</v>
       </c>
       <c r="K80" s="8"/>
       <c r="L80" s="27"/>

</xml_diff>

<commit_message>
added a serial command field for easy debugging
</commit_message>
<xml_diff>
--- a/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
+++ b/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgewi\Documents\Fynn\Projekte\Balloon\SpiCy-BEXUS\micorcontroller\Hardware\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83683B63-A460-44A4-8398-81CB5F3B9D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86BBFD4-EB24-457C-A48D-1363D5F11AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF6BBEE3-69E0-44E7-9484-437EE6090CBD}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="1">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -48,20 +48,10 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="1"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
-    </bk>
-    <bk>
-      <rc t="1" v="1"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -139,9 +129,6 @@
     <t>VCC (ntc+)</t>
   </si>
   <si>
-    <t>VCCoff (5V)</t>
-  </si>
-  <si>
     <t>Voff</t>
   </si>
   <si>
@@ -179,6 +166,9 @@
   </si>
   <si>
     <t>Imax</t>
+  </si>
+  <si>
+    <t>VCCoff (ntc+)</t>
   </si>
 </sst>
 </file>
@@ -397,6 +387,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -407,7 +398,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Akzent1" xfId="2" builtinId="30"/>
@@ -594,67 +584,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>9.7057622154934596E-3</c:v>
+                  <c:v>0.39230345894769753</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2598343170930336E-2</c:v>
+                  <c:v>0.49048018759388973</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6199026494879216E-2</c:v>
+                  <c:v>0.60303659529858811</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0641773750447085E-2</c:v>
+                  <c:v>0.72902279053401942</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6077262528154194E-2</c:v>
+                  <c:v>0.86662462746166813</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2673267326732675E-2</c:v>
+                  <c:v>1.0132450331125828</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0614658906958374E-2</c:v>
+                  <c:v>1.1657013916233732</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0102932076940214E-2</c:v>
+                  <c:v>1.320509046695193</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.1355167729016405E-2</c:v>
+                  <c:v>1.4741986257697359</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.4602334994228317E-2</c:v>
+                  <c:v>1.6236084919337195</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0086845259037457E-2</c:v>
+                  <c:v>1.7661049272612774</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10805928325461811</c:v>
+                  <c:v>1.8997056668068197</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.1287742631616135</c:v>
+                  <c:v>2.0231073596596065</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.15248539102088868</c:v>
+                  <c:v>2.1356361372431936</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.17943935939032254</c:v>
+                  <c:v>2.2371490909132357</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.24398723123301194</c:v>
+                  <c:v>2.4084892935858049</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.42041498309160763</c:v>
+                  <c:v>2.6447989740851292</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.1208813163169407</c:v>
+                  <c:v>2.8898397681187618</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.9185089414779546</c:v>
+                  <c:v>2.9582317510499139</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.4953196431987865</c:v>
+                  <c:v>2.9811500210306527</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.8298416372353588</c:v>
+                  <c:v>2.9902586172520094</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1018,67 +1008,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>339004.20850329078</c:v>
+                  <c:v>33900.420850329079</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>260939.20543571829</c:v>
+                  <c:v>26093.920543571829</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>202715.94558742066</c:v>
+                  <c:v>20271.594558742065</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>158869.98210018285</c:v>
+                  <c:v>15886.998210018286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>125547.02526529272</c:v>
+                  <c:v>12554.70252652927</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80251.451786404679</c:v>
+                  <c:v>8025.1451786404677</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64864.408792131726</c:v>
+                  <c:v>6486.4408792131726</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52785.200532331801</c:v>
+                  <c:v>5278.5200532331801</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43234.540383425097</c:v>
+                  <c:v>4323.4540383425092</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35631.31937311287</c:v>
+                  <c:v>3563.1319373112869</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29538.792231522304</c:v>
+                  <c:v>2953.8792231522302</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24626.238651883828</c:v>
+                  <c:v>2462.6238651883828</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20641.417436165666</c:v>
+                  <c:v>2064.1417436165666</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17390.614028117034</c:v>
+                  <c:v>1739.0614028117036</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12525.297956467419</c:v>
+                  <c:v>1252.5297956467418</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6849.3872309991775</c:v>
+                  <c:v>684.93872309991775</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1944.1118805007284</c:v>
+                  <c:v>194.41118805007284</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>720.08580656277297</c:v>
+                  <c:v>72.008580656277303</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>322.47586356098327</c:v>
+                  <c:v>32.247586356098331</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>166.14299421502844</c:v>
+                  <c:v>16.614299421502842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1432,67 +1422,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-0.78058847556901312</c:v>
+                  <c:v>-1.5393082104604994E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.77480331365813937</c:v>
+                  <c:v>0.18096037518777941</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.76760194701024165</c:v>
+                  <c:v>0.40607319059717617</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.75871645249910591</c:v>
+                  <c:v>0.65804558106803879</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.74784547494369169</c:v>
+                  <c:v>0.93324925492333621</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.73465346534653464</c:v>
+                  <c:v>1.2264900662251657</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.71877068218608331</c:v>
+                  <c:v>1.5314027832467463</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.6997941358461196</c:v>
+                  <c:v>1.8410180933903859</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.67728966454196726</c:v>
+                  <c:v>2.148397251539472</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.65079533001154344</c:v>
+                  <c:v>2.4472169838674391</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.61982630948192519</c:v>
+                  <c:v>2.732209854522555</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.58388143349076382</c:v>
+                  <c:v>2.9994113336136392</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.54245147367677304</c:v>
+                  <c:v>3.2462147193192132</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.49502921795822269</c:v>
+                  <c:v>3.4712722744863873</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.44112128121935495</c:v>
+                  <c:v>3.6742981818264715</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.31202553753397616</c:v>
+                  <c:v>4.0169785871716099</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.0829966183215216E-2</c:v>
+                  <c:v>4.4895979481702586</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.4417626326338813</c:v>
+                  <c:v>4.9796795362375237</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.0370178829559089</c:v>
+                  <c:v>5.1164635020998279</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.1906392863975732</c:v>
+                  <c:v>5.1623000420613057</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.8596832744707177</c:v>
+                  <c:v>5.1805172345040189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3615,6 +3605,50 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>356644</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>104381</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411222</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>8697</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8446C86A-C491-293C-9486-B91AAD9823FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1122123" y="12412943"/>
+          <a:ext cx="4812729" cy="2461713"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3659,7 +3693,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -3667,23 +3701,15 @@
 V_{\text{out}} = \left(1+\frac{R_4}{R_2}\right) \left(\frac{v_{dd}}{1+\frac{R_{ntc}}{R_1}} - \frac{V_{cc}}{1+\frac{R_3}{R_2}}\right)_x000D_
 \]</v>
   </rv>
-  <rv s="1">
-    <v>1</v>
-    <v>5</v>
-  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
   <s t="_localImage">
     <k n="_rvRel:LocalImageIdentifier" t="i"/>
     <k n="CalcOrigin" t="i"/>
     <k n="Text" t="s"/>
-  </s>
-  <s t="_localImage">
-    <k n="_rvRel:LocalImageIdentifier" t="i"/>
-    <k n="CalcOrigin" t="i"/>
   </s>
 </rvStructures>
 </file>
@@ -3691,7 +3717,6 @@
 <file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
-  <rel r:id="rId2"/>
 </richValueRels>
 </file>
 
@@ -4014,8 +4039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F92C7C-F2BA-463C-A1E4-8CB622B0EF6B}">
   <dimension ref="B1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="75" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="73" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4113,7 +4138,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="26">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -4122,7 +4147,7 @@
       </c>
       <c r="H6" s="26">
         <f t="shared" ref="H6:H26" si="0">D$6*EXP(D$5*(1/(G6+273.15)-1/298.15))</f>
-        <v>339004.20850329078</v>
+        <v>33900.420850329079</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
@@ -4145,7 +4170,7 @@
       </c>
       <c r="H7" s="26">
         <f t="shared" si="0"/>
-        <v>260939.20543571829</v>
+        <v>26093.920543571829</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -4163,12 +4188,12 @@
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="26">
-        <f t="shared" ref="G8:G25" si="1">G7+5</f>
+        <f t="shared" ref="G8:G20" si="1">G7+5</f>
         <v>10</v>
       </c>
       <c r="H8" s="26">
         <f t="shared" si="0"/>
-        <v>202715.94558742066</v>
+        <v>20271.594558742065</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
@@ -4191,7 +4216,7 @@
       </c>
       <c r="H9" s="26">
         <f t="shared" si="0"/>
-        <v>158869.98210018285</v>
+        <v>15886.998210018286</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -4214,7 +4239,7 @@
       </c>
       <c r="H10" s="26">
         <f t="shared" si="0"/>
-        <v>125547.02526529272</v>
+        <v>12554.70252652927</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -4239,7 +4264,7 @@
       </c>
       <c r="H11" s="26">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -4262,7 +4287,7 @@
       </c>
       <c r="H12" s="26">
         <f t="shared" si="0"/>
-        <v>80251.451786404679</v>
+        <v>8025.1451786404677</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
@@ -4285,7 +4310,7 @@
       </c>
       <c r="H13" s="26">
         <f t="shared" si="0"/>
-        <v>64864.408792131726</v>
+        <v>6486.4408792131726</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -4308,7 +4333,7 @@
       </c>
       <c r="H14" s="26">
         <f t="shared" si="0"/>
-        <v>52785.200532331801</v>
+        <v>5278.5200532331801</v>
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -4331,7 +4356,7 @@
       </c>
       <c r="H15" s="26">
         <f t="shared" si="0"/>
-        <v>43234.540383425097</v>
+        <v>4323.4540383425092</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -4354,7 +4379,7 @@
       </c>
       <c r="H16" s="26">
         <f t="shared" si="0"/>
-        <v>35631.31937311287</v>
+        <v>3563.1319373112869</v>
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -4377,7 +4402,7 @@
       </c>
       <c r="H17" s="26">
         <f t="shared" si="0"/>
-        <v>29538.792231522304</v>
+        <v>2953.8792231522302</v>
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -4400,7 +4425,7 @@
       </c>
       <c r="H18" s="26">
         <f t="shared" si="0"/>
-        <v>24626.238651883828</v>
+        <v>2462.6238651883828</v>
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -4425,7 +4450,7 @@
       </c>
       <c r="H19" s="26">
         <f t="shared" si="0"/>
-        <v>20641.417436165666</v>
+        <v>2064.1417436165666</v>
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -4448,7 +4473,7 @@
       </c>
       <c r="H20" s="26">
         <f t="shared" si="0"/>
-        <v>17390.614028117034</v>
+        <v>1739.0614028117036</v>
       </c>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -4470,7 +4495,7 @@
       </c>
       <c r="H21" s="26">
         <f t="shared" si="0"/>
-        <v>12525.297956467419</v>
+        <v>1252.5297956467418</v>
       </c>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -4492,7 +4517,7 @@
       </c>
       <c r="H22" s="26">
         <f t="shared" si="0"/>
-        <v>6849.3872309991775</v>
+        <v>684.93872309991775</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -4514,7 +4539,7 @@
       </c>
       <c r="H23" s="26">
         <f t="shared" si="0"/>
-        <v>1944.1118805007284</v>
+        <v>194.41118805007284</v>
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -4536,7 +4561,7 @@
       </c>
       <c r="H24" s="26">
         <f t="shared" si="0"/>
-        <v>720.08580656277297</v>
+        <v>72.008580656277303</v>
       </c>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -4558,7 +4583,7 @@
       </c>
       <c r="H25" s="26">
         <f t="shared" si="0"/>
-        <v>322.47586356098327</v>
+        <v>32.247586356098331</v>
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -4580,7 +4605,7 @@
       </c>
       <c r="H26" s="26">
         <f t="shared" si="0"/>
-        <v>166.14299421502844</v>
+        <v>16.614299421502842</v>
       </c>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -4698,7 +4723,7 @@
       </c>
       <c r="J33" s="26">
         <f>D34/(D35+H26)*1000</f>
-        <v>2.8298416372353588</v>
+        <v>0.58632521906902146</v>
       </c>
       <c r="K33" s="22"/>
       <c r="L33" s="20"/>
@@ -4712,8 +4737,8 @@
       <c r="C34" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="31">
-        <v>3.3</v>
+      <c r="D34" s="27">
+        <v>3</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="26">
@@ -4722,7 +4747,7 @@
       </c>
       <c r="G34" s="26">
         <f>D$34*(D$35/(D$35+H6))</f>
-        <v>9.7057622154934596E-3</v>
+        <v>0.39230345894769753</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="26" t="s">
@@ -4730,7 +4755,7 @@
       </c>
       <c r="J34" s="26">
         <f>1000*D34/(D35+H12)</f>
-        <v>4.0614658906958374E-2</v>
+        <v>0.22856890031830845</v>
       </c>
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
@@ -4745,7 +4770,7 @@
         <v>10</v>
       </c>
       <c r="D35" s="26">
-        <v>1000</v>
+        <v>5100</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="26">
@@ -4754,7 +4779,7 @@
       </c>
       <c r="G35" s="26">
         <f t="shared" ref="G35:G54" si="3">D$34*(D$35/(D$35+H7))</f>
-        <v>1.2598343170930336E-2</v>
+        <v>0.49048018759388973</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="26" t="s">
@@ -4762,7 +4787,7 @@
       </c>
       <c r="J35" s="26">
         <f>1000*(G41-G39)/10</f>
-        <v>1.7429664750207539</v>
+        <v>30.726401358261011</v>
       </c>
       <c r="K35" s="20"/>
       <c r="L35" s="20"/>
@@ -4782,11 +4807,11 @@
       </c>
       <c r="G36" s="26">
         <f t="shared" si="3"/>
-        <v>1.6199026494879216E-2</v>
+        <v>0.60303659529858811</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J36" s="26">
         <f>1000*3/POWER(2,D65)</f>
@@ -4810,15 +4835,15 @@
       </c>
       <c r="G37" s="26">
         <f t="shared" si="3"/>
-        <v>2.0641773750447085E-2</v>
+        <v>0.72902279053401942</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J37" s="26">
         <f>J36/J35</f>
-        <v>0.42021569863601588</v>
+        <v>2.3836890837302144E-2</v>
       </c>
       <c r="K37" s="20"/>
       <c r="L37" s="20"/>
@@ -4838,7 +4863,7 @@
       </c>
       <c r="G38" s="26">
         <f t="shared" si="3"/>
-        <v>2.6077262528154194E-2</v>
+        <v>0.86662462746166813</v>
       </c>
       <c r="H38" s="22"/>
       <c r="I38" s="20"/>
@@ -4861,7 +4886,7 @@
       </c>
       <c r="G39" s="26">
         <f t="shared" si="3"/>
-        <v>3.2673267326732675E-2</v>
+        <v>1.0132450331125828</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="20"/>
@@ -4884,7 +4909,7 @@
       </c>
       <c r="G40" s="26">
         <f t="shared" si="3"/>
-        <v>4.0614658906958374E-2</v>
+        <v>1.1657013916233732</v>
       </c>
       <c r="H40" s="22"/>
       <c r="I40" s="20"/>
@@ -4907,7 +4932,7 @@
       </c>
       <c r="G41" s="26">
         <f t="shared" si="3"/>
-        <v>5.0102932076940214E-2</v>
+        <v>1.320509046695193</v>
       </c>
       <c r="H41" s="22"/>
       <c r="I41" s="20"/>
@@ -4930,7 +4955,7 @@
       </c>
       <c r="G42" s="26">
         <f t="shared" si="3"/>
-        <v>6.1355167729016405E-2</v>
+        <v>1.4741986257697359</v>
       </c>
       <c r="H42" s="22"/>
       <c r="I42" s="20"/>
@@ -4953,7 +4978,7 @@
       </c>
       <c r="G43" s="26">
         <f t="shared" si="3"/>
-        <v>7.4602334994228317E-2</v>
+        <v>1.6236084919337195</v>
       </c>
       <c r="H43" s="22"/>
       <c r="I43" s="20"/>
@@ -4976,7 +5001,7 @@
       </c>
       <c r="G44" s="26">
         <f t="shared" si="3"/>
-        <v>9.0086845259037457E-2</v>
+        <v>1.7661049272612774</v>
       </c>
       <c r="H44" s="22"/>
       <c r="I44" s="20"/>
@@ -4999,7 +5024,7 @@
       </c>
       <c r="G45" s="26">
         <f t="shared" si="3"/>
-        <v>0.10805928325461811</v>
+        <v>1.8997056668068197</v>
       </c>
       <c r="H45" s="22"/>
       <c r="I45" s="20"/>
@@ -5022,7 +5047,7 @@
       </c>
       <c r="G46" s="26">
         <f t="shared" si="3"/>
-        <v>0.1287742631616135</v>
+        <v>2.0231073596596065</v>
       </c>
       <c r="H46" s="22"/>
       <c r="I46" s="20"/>
@@ -5045,7 +5070,7 @@
       </c>
       <c r="G47" s="26">
         <f t="shared" si="3"/>
-        <v>0.15248539102088868</v>
+        <v>2.1356361372431936</v>
       </c>
       <c r="H47" s="22"/>
       <c r="I47" s="20"/>
@@ -5068,7 +5093,7 @@
       </c>
       <c r="G48" s="26">
         <f t="shared" si="3"/>
-        <v>0.17943935939032254</v>
+        <v>2.2371490909132357</v>
       </c>
       <c r="H48" s="22"/>
       <c r="I48" s="20"/>
@@ -5091,7 +5116,7 @@
       </c>
       <c r="G49" s="26">
         <f>D$34*(D$35/(D$35+H21))</f>
-        <v>0.24398723123301194</v>
+        <v>2.4084892935858049</v>
       </c>
       <c r="H49" s="22"/>
       <c r="I49" s="20"/>
@@ -5114,7 +5139,7 @@
       </c>
       <c r="G50" s="26">
         <f t="shared" si="3"/>
-        <v>0.42041498309160763</v>
+        <v>2.6447989740851292</v>
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="20"/>
@@ -5137,7 +5162,7 @@
       </c>
       <c r="G51" s="26">
         <f t="shared" si="3"/>
-        <v>1.1208813163169407</v>
+        <v>2.8898397681187618</v>
       </c>
       <c r="H51" s="22"/>
       <c r="I51" s="20"/>
@@ -5160,7 +5185,7 @@
       </c>
       <c r="G52" s="26">
         <f t="shared" si="3"/>
-        <v>1.9185089414779546</v>
+        <v>2.9582317510499139</v>
       </c>
       <c r="H52" s="22"/>
       <c r="I52" s="20"/>
@@ -5183,7 +5208,7 @@
       </c>
       <c r="G53" s="26">
         <f t="shared" si="3"/>
-        <v>2.4953196431987865</v>
+        <v>2.9811500210306527</v>
       </c>
       <c r="H53" s="22"/>
       <c r="I53" s="20"/>
@@ -5206,7 +5231,7 @@
       </c>
       <c r="G54" s="26">
         <f t="shared" si="3"/>
-        <v>2.8298416372353588</v>
+        <v>2.9902586172520094</v>
       </c>
       <c r="H54" s="22"/>
       <c r="I54" s="20"/>
@@ -5290,14 +5315,14 @@
       </c>
       <c r="K59" s="8"/>
       <c r="L59" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M59" s="26">
         <f>G60/(G61+K52)*1000</f>
         <v>0</v>
       </c>
       <c r="N59" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O59" s="8"/>
       <c r="P59" s="9"/>
@@ -5312,28 +5337,28 @@
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G60" s="26"/>
       <c r="H60" s="8"/>
       <c r="I60" s="26">
-        <f>F34</f>
+        <f t="shared" ref="I60:I80" si="22">F34</f>
         <v>0</v>
       </c>
       <c r="J60" s="26">
-        <f>D$60*(G34-D$61)</f>
-        <v>-0.78058847556901312</v>
+        <f t="shared" ref="J60:J80" si="23">D$60*(G34-D$61)</f>
+        <v>-1.5393082104604994E-2</v>
       </c>
       <c r="K60" s="8"/>
       <c r="L60" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M60" s="26">
         <f>1000*G60/(G61+K38)</f>
         <v>0</v>
       </c>
       <c r="N60" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O60" s="8"/>
       <c r="P60" s="9"/>
@@ -5341,7 +5366,7 @@
     <row r="61" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B61" s="7"/>
       <c r="C61" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D61" s="26">
         <v>0.4</v>
@@ -5352,16 +5377,16 @@
       </c>
       <c r="G61" s="26">
         <f>(D62-D61)*D64/D61</f>
-        <v>72500</v>
+        <v>65000</v>
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="26">
-        <f>F35</f>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
       <c r="J61" s="26">
-        <f>D$60*(G35-D$61)</f>
-        <v>-0.77480331365813937</v>
+        <f t="shared" si="23"/>
+        <v>0.18096037518777941</v>
       </c>
       <c r="K61" s="8"/>
       <c r="L61" s="26" t="s">
@@ -5369,10 +5394,10 @@
       </c>
       <c r="M61" s="26">
         <f>1000*(J67-J65)/10</f>
-        <v>3.4859329500415037</v>
+        <v>61.452802716522022</v>
       </c>
       <c r="N61" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O61" s="8"/>
       <c r="P61" s="9"/>
@@ -5380,10 +5405,10 @@
     <row r="62" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B62" s="7"/>
       <c r="C62" s="26" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D62" s="26">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="26" t="s">
@@ -5395,23 +5420,23 @@
       </c>
       <c r="H62" s="8"/>
       <c r="I62" s="26">
-        <f>F36</f>
+        <f t="shared" si="22"/>
         <v>10</v>
       </c>
       <c r="J62" s="26">
-        <f>D$60*(G36-D$61)</f>
-        <v>-0.76760194701024165</v>
+        <f t="shared" si="23"/>
+        <v>0.40607319059717617</v>
       </c>
       <c r="K62" s="8"/>
       <c r="L62" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M62" s="26">
         <f>1000*3/POWER(2,D65)</f>
         <v>0.732421875</v>
       </c>
       <c r="N62" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O62" s="8"/>
       <c r="P62" s="9"/>
@@ -5423,30 +5448,30 @@
       </c>
       <c r="D63" s="26">
         <f>D35</f>
-        <v>1000</v>
+        <v>5100</v>
       </c>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
       <c r="I63" s="26">
-        <f>F37</f>
+        <f t="shared" si="22"/>
         <v>15</v>
       </c>
       <c r="J63" s="26">
-        <f>D$60*(G37-D$61)</f>
-        <v>-0.75871645249910591</v>
+        <f t="shared" si="23"/>
+        <v>0.65804558106803879</v>
       </c>
       <c r="K63" s="8"/>
       <c r="L63" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M63" s="26">
         <f>M62/M61</f>
-        <v>0.21010784931800819</v>
+        <v>1.1918445418651072E-2</v>
       </c>
       <c r="N63" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O63" s="8"/>
       <c r="P63" s="9"/>
@@ -5459,19 +5484,19 @@
       <c r="D64" s="26">
         <v>10000</v>
       </c>
-      <c r="E64" s="29" t="e" vm="1">
+      <c r="E64" s="30" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="30"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="31"/>
       <c r="I64" s="26">
-        <f>F38</f>
+        <f t="shared" si="22"/>
         <v>20</v>
       </c>
       <c r="J64" s="26">
-        <f>D$60*(G38-D$61)</f>
-        <v>-0.74784547494369169</v>
+        <f t="shared" si="23"/>
+        <v>0.93324925492333621</v>
       </c>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
@@ -5483,55 +5508,55 @@
     <row r="65" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B65" s="7"/>
       <c r="C65" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D65" s="26">
         <v>12</v>
       </c>
-      <c r="E65" s="29"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="28"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="31"/>
       <c r="I65" s="26">
-        <f>F39</f>
+        <f t="shared" si="22"/>
         <v>25</v>
       </c>
       <c r="J65" s="26">
-        <f>D$60*(G39-D$61)</f>
-        <v>-0.73465346534653464</v>
+        <f t="shared" si="23"/>
+        <v>1.2264900662251657</v>
       </c>
       <c r="K65" s="8"/>
-      <c r="L65" s="27"/>
-      <c r="M65" s="27"/>
-      <c r="N65" s="27"/>
-      <c r="O65" s="27"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="28"/>
+      <c r="N65" s="28"/>
+      <c r="O65" s="28"/>
       <c r="P65" s="9"/>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B66" s="7"/>
       <c r="C66" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D66" s="26">
         <v>3</v>
       </c>
-      <c r="E66" s="29"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
-      <c r="H66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="28"/>
+      <c r="H66" s="31"/>
       <c r="I66" s="26">
-        <f>F40</f>
+        <f t="shared" si="22"/>
         <v>30</v>
       </c>
       <c r="J66" s="26">
-        <f>D$60*(G40-D$61)</f>
-        <v>-0.71877068218608331</v>
+        <f t="shared" si="23"/>
+        <v>1.5314027832467463</v>
       </c>
       <c r="K66" s="8"/>
-      <c r="L66" s="27"/>
-      <c r="M66" s="27"/>
-      <c r="N66" s="27"/>
-      <c r="O66" s="27"/>
+      <c r="L66" s="28"/>
+      <c r="M66" s="28"/>
+      <c r="N66" s="28"/>
+      <c r="O66" s="28"/>
       <c r="P66" s="9"/>
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.35">
@@ -5543,404 +5568,402 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
       <c r="I67" s="26">
-        <f>F41</f>
+        <f t="shared" si="22"/>
         <v>35</v>
       </c>
       <c r="J67" s="26">
-        <f>D$60*(G41-D$61)</f>
-        <v>-0.6997941358461196</v>
+        <f t="shared" si="23"/>
+        <v>1.8410180933903859</v>
       </c>
       <c r="K67" s="8"/>
-      <c r="L67" s="27"/>
-      <c r="M67" s="27"/>
-      <c r="N67" s="27"/>
-      <c r="O67" s="27"/>
+      <c r="L67" s="28"/>
+      <c r="M67" s="28"/>
+      <c r="N67" s="28"/>
+      <c r="O67" s="28"/>
       <c r="P67" s="9"/>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B68" s="7"/>
-      <c r="C68" s="28" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="D68" s="28"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="28"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="29"/>
       <c r="H68" s="8"/>
       <c r="I68" s="26">
-        <f>F42</f>
+        <f t="shared" si="22"/>
         <v>40</v>
       </c>
       <c r="J68" s="26">
-        <f>D$60*(G42-D$61)</f>
-        <v>-0.67728966454196726</v>
+        <f t="shared" si="23"/>
+        <v>2.148397251539472</v>
       </c>
       <c r="K68" s="8"/>
-      <c r="L68" s="27"/>
-      <c r="M68" s="27"/>
-      <c r="N68" s="27"/>
-      <c r="O68" s="27"/>
+      <c r="L68" s="28"/>
+      <c r="M68" s="28"/>
+      <c r="N68" s="28"/>
+      <c r="O68" s="28"/>
       <c r="P68" s="9"/>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B69" s="7"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
       <c r="H69" s="8"/>
       <c r="I69" s="26">
-        <f>F43</f>
+        <f t="shared" si="22"/>
         <v>45</v>
       </c>
       <c r="J69" s="26">
-        <f>D$60*(G43-D$61)</f>
-        <v>-0.65079533001154344</v>
+        <f t="shared" si="23"/>
+        <v>2.4472169838674391</v>
       </c>
       <c r="K69" s="8"/>
-      <c r="L69" s="27"/>
-      <c r="M69" s="27"/>
-      <c r="N69" s="27"/>
-      <c r="O69" s="27"/>
+      <c r="L69" s="28"/>
+      <c r="M69" s="28"/>
+      <c r="N69" s="28"/>
+      <c r="O69" s="28"/>
       <c r="P69" s="9"/>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B70" s="7"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="28"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="29"/>
       <c r="H70" s="8"/>
       <c r="I70" s="26">
-        <f>F44</f>
+        <f t="shared" si="22"/>
         <v>50</v>
       </c>
       <c r="J70" s="26">
-        <f>D$60*(G44-D$61)</f>
-        <v>-0.61982630948192519</v>
+        <f t="shared" si="23"/>
+        <v>2.732209854522555</v>
       </c>
       <c r="K70" s="8"/>
-      <c r="L70" s="27"/>
-      <c r="M70" s="27"/>
-      <c r="N70" s="27"/>
-      <c r="O70" s="27"/>
+      <c r="L70" s="28"/>
+      <c r="M70" s="28"/>
+      <c r="N70" s="28"/>
+      <c r="O70" s="28"/>
       <c r="P70" s="9"/>
     </row>
     <row r="71" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B71" s="7"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="28"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
       <c r="H71" s="8"/>
       <c r="I71" s="26">
-        <f>F45</f>
+        <f t="shared" si="22"/>
         <v>55</v>
       </c>
       <c r="J71" s="26">
-        <f>D$60*(G45-D$61)</f>
-        <v>-0.58388143349076382</v>
+        <f t="shared" si="23"/>
+        <v>2.9994113336136392</v>
       </c>
       <c r="K71" s="8"/>
-      <c r="L71" s="27"/>
-      <c r="M71" s="27"/>
-      <c r="N71" s="27"/>
-      <c r="O71" s="27"/>
+      <c r="L71" s="28"/>
+      <c r="M71" s="28"/>
+      <c r="N71" s="28"/>
+      <c r="O71" s="28"/>
       <c r="P71" s="9"/>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B72" s="7"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="28"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="29"/>
       <c r="H72" s="8"/>
       <c r="I72" s="26">
-        <f>F46</f>
+        <f t="shared" si="22"/>
         <v>60</v>
       </c>
       <c r="J72" s="26">
-        <f>D$60*(G46-D$61)</f>
-        <v>-0.54245147367677304</v>
+        <f t="shared" si="23"/>
+        <v>3.2462147193192132</v>
       </c>
       <c r="K72" s="8"/>
-      <c r="L72" s="27"/>
-      <c r="M72" s="27"/>
-      <c r="N72" s="27"/>
-      <c r="O72" s="27"/>
+      <c r="L72" s="28"/>
+      <c r="M72" s="28"/>
+      <c r="N72" s="28"/>
+      <c r="O72" s="28"/>
       <c r="P72" s="9"/>
     </row>
     <row r="73" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B73" s="7"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
-      <c r="E73" s="28"/>
-      <c r="F73" s="28"/>
-      <c r="G73" s="28"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
       <c r="H73" s="8"/>
       <c r="I73" s="26">
-        <f>F47</f>
+        <f t="shared" si="22"/>
         <v>65</v>
       </c>
       <c r="J73" s="26">
-        <f>D$60*(G47-D$61)</f>
-        <v>-0.49502921795822269</v>
+        <f t="shared" si="23"/>
+        <v>3.4712722744863873</v>
       </c>
       <c r="K73" s="8"/>
-      <c r="L73" s="27"/>
-      <c r="M73" s="27"/>
-      <c r="N73" s="27"/>
-      <c r="O73" s="27"/>
+      <c r="L73" s="28"/>
+      <c r="M73" s="28"/>
+      <c r="N73" s="28"/>
+      <c r="O73" s="28"/>
       <c r="P73" s="9"/>
     </row>
     <row r="74" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B74" s="7"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="28"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
       <c r="H74" s="8"/>
       <c r="I74" s="26">
-        <f>F48</f>
+        <f t="shared" si="22"/>
         <v>70</v>
       </c>
       <c r="J74" s="26">
-        <f>D$60*(G48-D$61)</f>
-        <v>-0.44112128121935495</v>
+        <f t="shared" si="23"/>
+        <v>3.6742981818264715</v>
       </c>
       <c r="K74" s="8"/>
-      <c r="L74" s="27"/>
-      <c r="M74" s="27"/>
-      <c r="N74" s="27"/>
-      <c r="O74" s="27"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="28"/>
+      <c r="N74" s="28"/>
+      <c r="O74" s="28"/>
       <c r="P74" s="9"/>
     </row>
     <row r="75" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B75" s="7"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
       <c r="H75" s="8"/>
       <c r="I75" s="26">
-        <f>F49</f>
+        <f t="shared" si="22"/>
         <v>80</v>
       </c>
       <c r="J75" s="26">
-        <f>D$60*(G49-D$61)</f>
-        <v>-0.31202553753397616</v>
+        <f t="shared" si="23"/>
+        <v>4.0169785871716099</v>
       </c>
       <c r="K75" s="8"/>
-      <c r="L75" s="27"/>
-      <c r="M75" s="27"/>
-      <c r="N75" s="27"/>
-      <c r="O75" s="27"/>
+      <c r="L75" s="28"/>
+      <c r="M75" s="28"/>
+      <c r="N75" s="28"/>
+      <c r="O75" s="28"/>
       <c r="P75" s="9"/>
     </row>
     <row r="76" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B76" s="7"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="28"/>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="28"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
       <c r="H76" s="8"/>
       <c r="I76" s="26">
-        <f>F50</f>
+        <f t="shared" si="22"/>
         <v>100</v>
       </c>
       <c r="J76" s="26">
-        <f>D$60*(G50-D$61)</f>
-        <v>4.0829966183215216E-2</v>
+        <f t="shared" si="23"/>
+        <v>4.4895979481702586</v>
       </c>
       <c r="K76" s="8"/>
-      <c r="L76" s="27"/>
-      <c r="M76" s="27"/>
-      <c r="N76" s="27"/>
-      <c r="O76" s="27"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="28"/>
+      <c r="N76" s="28"/>
+      <c r="O76" s="28"/>
       <c r="P76" s="9"/>
     </row>
     <row r="77" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B77" s="7"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="28"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="28"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
       <c r="H77" s="8"/>
       <c r="I77" s="26">
-        <f>F51</f>
+        <f t="shared" si="22"/>
         <v>150</v>
       </c>
       <c r="J77" s="26">
-        <f>D$60*(G51-D$61)</f>
-        <v>1.4417626326338813</v>
+        <f t="shared" si="23"/>
+        <v>4.9796795362375237</v>
       </c>
       <c r="K77" s="8"/>
-      <c r="L77" s="27"/>
-      <c r="M77" s="27"/>
-      <c r="N77" s="27"/>
-      <c r="O77" s="27"/>
+      <c r="L77" s="28"/>
+      <c r="M77" s="28"/>
+      <c r="N77" s="28"/>
+      <c r="O77" s="28"/>
       <c r="P77" s="9"/>
     </row>
     <row r="78" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B78" s="7"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="28"/>
-      <c r="E78" s="28"/>
-      <c r="F78" s="28"/>
-      <c r="G78" s="28"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
       <c r="H78" s="8"/>
       <c r="I78" s="26">
-        <f>F52</f>
+        <f t="shared" si="22"/>
         <v>200</v>
       </c>
       <c r="J78" s="26">
-        <f>D$60*(G52-D$61)</f>
-        <v>3.0370178829559089</v>
+        <f t="shared" si="23"/>
+        <v>5.1164635020998279</v>
       </c>
       <c r="K78" s="8"/>
-      <c r="L78" s="27"/>
-      <c r="M78" s="27"/>
-      <c r="N78" s="27"/>
-      <c r="O78" s="27"/>
+      <c r="L78" s="28"/>
+      <c r="M78" s="28"/>
+      <c r="N78" s="28"/>
+      <c r="O78" s="28"/>
       <c r="P78" s="9"/>
     </row>
     <row r="79" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B79" s="7"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="28"/>
-      <c r="E79" s="28"/>
-      <c r="F79" s="28"/>
-      <c r="G79" s="28"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="29"/>
       <c r="H79" s="8"/>
       <c r="I79" s="26">
-        <f>F53</f>
+        <f t="shared" si="22"/>
         <v>250</v>
       </c>
       <c r="J79" s="26">
-        <f>D$60*(G53-D$61)</f>
-        <v>4.1906392863975732</v>
+        <f t="shared" si="23"/>
+        <v>5.1623000420613057</v>
       </c>
       <c r="K79" s="8"/>
-      <c r="L79" s="27"/>
-      <c r="M79" s="27"/>
-      <c r="N79" s="27"/>
-      <c r="O79" s="27"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="28"/>
+      <c r="N79" s="28"/>
+      <c r="O79" s="28"/>
       <c r="P79" s="9"/>
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B80" s="7"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="28"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
       <c r="H80" s="8"/>
       <c r="I80" s="26">
-        <f>F54</f>
+        <f t="shared" si="22"/>
         <v>300</v>
       </c>
       <c r="J80" s="26">
-        <f>D$60*(G54-D$61)</f>
-        <v>4.8596832744707177</v>
+        <f t="shared" si="23"/>
+        <v>5.1805172345040189</v>
       </c>
       <c r="K80" s="8"/>
-      <c r="L80" s="27"/>
-      <c r="M80" s="27"/>
-      <c r="N80" s="27"/>
-      <c r="O80" s="27"/>
+      <c r="L80" s="28"/>
+      <c r="M80" s="28"/>
+      <c r="N80" s="28"/>
+      <c r="O80" s="28"/>
       <c r="P80" s="9"/>
     </row>
     <row r="81" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B81" s="7"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="28"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="29"/>
       <c r="H81" s="8"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
-      <c r="L81" s="27"/>
-      <c r="M81" s="27"/>
-      <c r="N81" s="27"/>
-      <c r="O81" s="27"/>
+      <c r="L81" s="28"/>
+      <c r="M81" s="28"/>
+      <c r="N81" s="28"/>
+      <c r="O81" s="28"/>
       <c r="P81" s="9"/>
     </row>
     <row r="82" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B82" s="7"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
-      <c r="E82" s="28"/>
-      <c r="F82" s="28"/>
-      <c r="G82" s="28"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="29"/>
+      <c r="G82" s="29"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
       <c r="K82" s="8"/>
-      <c r="L82" s="27"/>
-      <c r="M82" s="27"/>
-      <c r="N82" s="27"/>
-      <c r="O82" s="27"/>
+      <c r="L82" s="28"/>
+      <c r="M82" s="28"/>
+      <c r="N82" s="28"/>
+      <c r="O82" s="28"/>
       <c r="P82" s="9"/>
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B83" s="7"/>
-      <c r="C83" s="28"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="28"/>
-      <c r="F83" s="28"/>
-      <c r="G83" s="28"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="29"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
       <c r="K83" s="8"/>
-      <c r="L83" s="27"/>
-      <c r="M83" s="27"/>
-      <c r="N83" s="27"/>
-      <c r="O83" s="27"/>
+      <c r="L83" s="28"/>
+      <c r="M83" s="28"/>
+      <c r="N83" s="28"/>
+      <c r="O83" s="28"/>
       <c r="P83" s="9"/>
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B84" s="7"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="28"/>
-      <c r="E84" s="28"/>
-      <c r="F84" s="28"/>
-      <c r="G84" s="28"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="29"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
-      <c r="L84" s="27"/>
-      <c r="M84" s="27"/>
-      <c r="N84" s="27"/>
-      <c r="O84" s="27"/>
+      <c r="L84" s="28"/>
+      <c r="M84" s="28"/>
+      <c r="N84" s="28"/>
+      <c r="O84" s="28"/>
       <c r="P84" s="9"/>
     </row>
     <row r="85" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B85" s="7"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="28"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="28"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
       <c r="K85" s="8"/>
-      <c r="L85" s="27"/>
-      <c r="M85" s="27"/>
-      <c r="N85" s="27"/>
-      <c r="O85" s="27"/>
+      <c r="L85" s="28"/>
+      <c r="M85" s="28"/>
+      <c r="N85" s="28"/>
+      <c r="O85" s="28"/>
       <c r="P85" s="9"/>
     </row>
     <row r="86" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Switch to header BASED C file system {headache incomming}
</commit_message>
<xml_diff>
--- a/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
+++ b/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgewi\Documents\Fynn\Projekte\Balloon\SpiCy-BEXUS\micorcontroller\Hardware\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86BBFD4-EB24-457C-A48D-1363D5F11AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E3548B-38D9-479B-9434-90BBA39CFD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF6BBEE3-69E0-44E7-9484-437EE6090CBD}"/>
   </bookViews>
@@ -4037,10 +4037,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F92C7C-F2BA-463C-A1E4-8CB622B0EF6B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="73" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:P86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5990,7 +5993,7 @@
     <mergeCell ref="E64:H66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="66" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed debug to level based debug and started writing driver for FD-OEM Module
</commit_message>
<xml_diff>
--- a/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
+++ b/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgewi\Documents\Fynn\Projekte\Balloon\SpiCy-BEXUS\micorcontroller\Hardware\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E3548B-38D9-479B-9434-90BBA39CFD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C205370B-7270-4852-94DB-9FDE131A7C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF6BBEE3-69E0-44E7-9484-437EE6090CBD}"/>
   </bookViews>
@@ -4042,8 +4042,8 @@
   </sheetPr>
   <dimension ref="B1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:P86"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="123" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
trying to fix things
</commit_message>
<xml_diff>
--- a/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
+++ b/micorcontroller/Hardware/Calculations/NTC Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fgewi\Documents\Fynn\Projekte\Balloon\SpiCy-BEXUS\micorcontroller\Hardware\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C205370B-7270-4852-94DB-9FDE131A7C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7929E5BD-CBDA-48D0-A40C-8F00736C66C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FF6BBEE3-69E0-44E7-9484-437EE6090CBD}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Temperature</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>Imax</t>
-  </si>
-  <si>
-    <t>VCCoff (ntc+)</t>
   </si>
 </sst>
 </file>
@@ -359,7 +356,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -398,6 +395,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Akzent1" xfId="2" builtinId="30"/>
@@ -1422,67 +1420,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-1.5393082104604994E-2</c:v>
+                  <c:v>0.27329390740596615</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18096037518777941</c:v>
+                  <c:v>0.488897710386203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.40607319059717617</c:v>
+                  <c:v>0.73608041738372543</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65804558106803879</c:v>
+                  <c:v>1.0127559920370586</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93324925492333621</c:v>
+                  <c:v>1.3149404276743739</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2264900662251657</c:v>
+                  <c:v>1.6369303481856263</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5314027832467463</c:v>
+                  <c:v>1.9717364792994649</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8410180933903859</c:v>
+                  <c:v>2.3117062422381047</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.148397251539472</c:v>
+                  <c:v>2.6492206225177584</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4472169838674391</c:v>
+                  <c:v>2.9773364172883601</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.732209854522555</c:v>
+                  <c:v>3.2902697752378507</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9994113336136392</c:v>
+                  <c:v>3.5836674869379155</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2462147193192132</c:v>
+                  <c:v>3.8546672914755247</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.4712722744863873</c:v>
+                  <c:v>4.1017893205581224</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6742981818264715</c:v>
+                  <c:v>4.3247197355843978</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.0169785871716099</c:v>
+                  <c:v>4.7009962708592692</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.4895979481702586</c:v>
+                  <c:v>5.2199508795457046</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.9796795362375237</c:v>
+                  <c:v>5.7580796989458936</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.1164635020998279</c:v>
+                  <c:v>5.9082738622333633</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.1623000420613057</c:v>
+                  <c:v>5.95860418219526</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.1805172345040189</c:v>
+                  <c:v>5.978607374522162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3363,7 +3361,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>725026</xdr:colOff>
+      <xdr:colOff>717727</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>22169</xdr:rowOff>
     </xdr:to>
@@ -3407,7 +3405,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>165656</xdr:colOff>
+      <xdr:colOff>158357</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>19921</xdr:rowOff>
     </xdr:to>
@@ -3614,7 +3612,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>411222</xdr:colOff>
+      <xdr:colOff>294441</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>8697</xdr:rowOff>
     </xdr:to>
@@ -4042,16 +4040,20 @@
   </sheetPr>
   <dimension ref="B1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="123" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="87" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="13.26953125" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.54296875" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.1796875" customWidth="1"/>
     <col min="12" max="12" width="23.26953125" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -5335,8 +5337,8 @@
       <c r="C60" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="26">
-        <v>2</v>
+      <c r="D60" s="32">
+        <v>2.1960785</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="26" t="s">
@@ -5350,7 +5352,7 @@
       </c>
       <c r="J60" s="26">
         <f t="shared" ref="J60:J80" si="23">D$60*(G34-D$61)</f>
-        <v>-1.5393082104604994E-2</v>
+        <v>0.27329390740596615</v>
       </c>
       <c r="K60" s="8"/>
       <c r="L60" s="26" t="s">
@@ -5371,8 +5373,8 @@
       <c r="C61" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D61" s="26">
-        <v>0.4</v>
+      <c r="D61" s="27">
+        <v>0.26785713</v>
       </c>
       <c r="E61" s="8"/>
       <c r="F61" s="26" t="s">
@@ -5380,7 +5382,7 @@
       </c>
       <c r="G61" s="26">
         <f>(D62-D61)*D64/D61</f>
-        <v>65000</v>
+        <v>102000.00537600026</v>
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="26">
@@ -5389,7 +5391,7 @@
       </c>
       <c r="J61" s="26">
         <f t="shared" si="23"/>
-        <v>0.18096037518777941</v>
+        <v>0.488897710386203</v>
       </c>
       <c r="K61" s="8"/>
       <c r="L61" s="26" t="s">
@@ -5397,7 +5399,7 @@
       </c>
       <c r="M61" s="26">
         <f>1000*(J67-J65)/10</f>
-        <v>61.452802716522022</v>
+        <v>67.477589405247841</v>
       </c>
       <c r="N61" s="26" t="s">
         <v>32</v>
@@ -5408,7 +5410,7 @@
     <row r="62" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B62" s="7"/>
       <c r="C62" s="26" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D62" s="26">
         <v>3</v>
@@ -5419,7 +5421,7 @@
       </c>
       <c r="G62" s="26">
         <f>D64*(D60-1)</f>
-        <v>10000</v>
+        <v>11960.785</v>
       </c>
       <c r="H62" s="8"/>
       <c r="I62" s="26">
@@ -5428,7 +5430,7 @@
       </c>
       <c r="J62" s="26">
         <f t="shared" si="23"/>
-        <v>0.40607319059717617</v>
+        <v>0.73608041738372543</v>
       </c>
       <c r="K62" s="8"/>
       <c r="L62" s="26" t="s">
@@ -5463,7 +5465,7 @@
       </c>
       <c r="J63" s="26">
         <f t="shared" si="23"/>
-        <v>0.65804558106803879</v>
+        <v>1.0127559920370586</v>
       </c>
       <c r="K63" s="8"/>
       <c r="L63" s="26" t="s">
@@ -5471,7 +5473,7 @@
       </c>
       <c r="M63" s="26">
         <f>M62/M61</f>
-        <v>1.1918445418651072E-2</v>
+        <v>1.0854298167074687E-2</v>
       </c>
       <c r="N63" s="26" t="s">
         <v>30</v>
@@ -5499,7 +5501,7 @@
       </c>
       <c r="J64" s="26">
         <f t="shared" si="23"/>
-        <v>0.93324925492333621</v>
+        <v>1.3149404276743739</v>
       </c>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
@@ -5526,7 +5528,7 @@
       </c>
       <c r="J65" s="26">
         <f t="shared" si="23"/>
-        <v>1.2264900662251657</v>
+        <v>1.6369303481856263</v>
       </c>
       <c r="K65" s="8"/>
       <c r="L65" s="28"/>
@@ -5553,7 +5555,7 @@
       </c>
       <c r="J66" s="26">
         <f t="shared" si="23"/>
-        <v>1.5314027832467463</v>
+        <v>1.9717364792994649</v>
       </c>
       <c r="K66" s="8"/>
       <c r="L66" s="28"/>
@@ -5576,7 +5578,7 @@
       </c>
       <c r="J67" s="26">
         <f t="shared" si="23"/>
-        <v>1.8410180933903859</v>
+        <v>2.3117062422381047</v>
       </c>
       <c r="K67" s="8"/>
       <c r="L67" s="28"/>
@@ -5599,7 +5601,7 @@
       </c>
       <c r="J68" s="26">
         <f t="shared" si="23"/>
-        <v>2.148397251539472</v>
+        <v>2.6492206225177584</v>
       </c>
       <c r="K68" s="8"/>
       <c r="L68" s="28"/>
@@ -5622,7 +5624,7 @@
       </c>
       <c r="J69" s="26">
         <f t="shared" si="23"/>
-        <v>2.4472169838674391</v>
+        <v>2.9773364172883601</v>
       </c>
       <c r="K69" s="8"/>
       <c r="L69" s="28"/>
@@ -5645,7 +5647,7 @@
       </c>
       <c r="J70" s="26">
         <f t="shared" si="23"/>
-        <v>2.732209854522555</v>
+        <v>3.2902697752378507</v>
       </c>
       <c r="K70" s="8"/>
       <c r="L70" s="28"/>
@@ -5668,7 +5670,7 @@
       </c>
       <c r="J71" s="26">
         <f t="shared" si="23"/>
-        <v>2.9994113336136392</v>
+        <v>3.5836674869379155</v>
       </c>
       <c r="K71" s="8"/>
       <c r="L71" s="28"/>
@@ -5691,7 +5693,7 @@
       </c>
       <c r="J72" s="26">
         <f t="shared" si="23"/>
-        <v>3.2462147193192132</v>
+        <v>3.8546672914755247</v>
       </c>
       <c r="K72" s="8"/>
       <c r="L72" s="28"/>
@@ -5714,7 +5716,7 @@
       </c>
       <c r="J73" s="26">
         <f t="shared" si="23"/>
-        <v>3.4712722744863873</v>
+        <v>4.1017893205581224</v>
       </c>
       <c r="K73" s="8"/>
       <c r="L73" s="28"/>
@@ -5737,7 +5739,7 @@
       </c>
       <c r="J74" s="26">
         <f t="shared" si="23"/>
-        <v>3.6742981818264715</v>
+        <v>4.3247197355843978</v>
       </c>
       <c r="K74" s="8"/>
       <c r="L74" s="28"/>
@@ -5760,7 +5762,7 @@
       </c>
       <c r="J75" s="26">
         <f t="shared" si="23"/>
-        <v>4.0169785871716099</v>
+        <v>4.7009962708592692</v>
       </c>
       <c r="K75" s="8"/>
       <c r="L75" s="28"/>
@@ -5783,7 +5785,7 @@
       </c>
       <c r="J76" s="26">
         <f t="shared" si="23"/>
-        <v>4.4895979481702586</v>
+        <v>5.2199508795457046</v>
       </c>
       <c r="K76" s="8"/>
       <c r="L76" s="28"/>
@@ -5806,7 +5808,7 @@
       </c>
       <c r="J77" s="26">
         <f t="shared" si="23"/>
-        <v>4.9796795362375237</v>
+        <v>5.7580796989458936</v>
       </c>
       <c r="K77" s="8"/>
       <c r="L77" s="28"/>
@@ -5829,7 +5831,7 @@
       </c>
       <c r="J78" s="26">
         <f t="shared" si="23"/>
-        <v>5.1164635020998279</v>
+        <v>5.9082738622333633</v>
       </c>
       <c r="K78" s="8"/>
       <c r="L78" s="28"/>
@@ -5852,7 +5854,7 @@
       </c>
       <c r="J79" s="26">
         <f t="shared" si="23"/>
-        <v>5.1623000420613057</v>
+        <v>5.95860418219526</v>
       </c>
       <c r="K79" s="8"/>
       <c r="L79" s="28"/>
@@ -5875,7 +5877,7 @@
       </c>
       <c r="J80" s="26">
         <f t="shared" si="23"/>
-        <v>5.1805172345040189</v>
+        <v>5.978607374522162</v>
       </c>
       <c r="K80" s="8"/>
       <c r="L80" s="28"/>

</xml_diff>